<commit_message>
New Commit 1 November
</commit_message>
<xml_diff>
--- a/SCTestData/data.xlsx
+++ b/SCTestData/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashine_a\Katalon Studio\SafetyChain\SCTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Data\SafetyChain-Test-Automation-Katalon\SCTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9E5B75-C7E4-4915-9CEB-13607A577460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1724257C-F393-4432-87B8-0509758E9E15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{46E2E1DA-1FC9-488C-935C-41E78C701628}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,278 +30,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>FormName</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_1540556466641</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_1540564284224</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_1540564494602</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_1540564730363</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_1540789513614</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540789770277</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540790038659</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540792707579</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540792907903</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540793643378</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540793731454</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540794941802</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540795181630</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540795407815</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540796297808</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540797088846</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540797323670</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540797546890</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540797898229</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540798156606</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540798415236</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540798807966</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540799056503</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540800978537</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540801113785</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540801285289</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540801682703</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540801934991</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540802177096</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540802562892</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540802797720</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540803020971</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540803807203</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540804064173</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540804287278</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540804735680</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540804850703</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540805092576</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540805309313</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540806044828</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540807883386</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540808134550</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540808351591</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540808810744</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540809079628</t>
-  </si>
-  <si>
-    <t>AUTO_29OCT_TOOL_KAT_1540809325735</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540889810289</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540891420271</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540891686239</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540891906051</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540892353385</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540892612327</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540892854267</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540893266411</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540893458319</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540893699787</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540893986430</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540894238982</t>
-  </si>
-  <si>
-    <t>AUTO_30OCT_TOOL_KAT_1540894475278</t>
-  </si>
-  <si>
-    <t>AUTO_31OCT_TOOL_KAT_1540977026645</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-14:53:31</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-14:57:31</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:01:21</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:09:10</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:13:45</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:19:26</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:25:36</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:28:47</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_31/10/2018-15:32:37</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-11:57:22</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:00:09</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:00:35</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:05:05</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:07:34</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:12:55</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:16:19</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:19:14</t>
   </si>
   <si>
     <t>AUTO_TOOL_KAT_01/11/2018-12:20:27</t>
   </si>
   <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:23:11</t>
+    <t>AUTO_TOOL_KAT_TASK01/11/2018-14:59:49</t>
   </si>
   <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:24:25</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:26:50</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:32:46</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:34:55</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:36:09</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:37:40</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:39:03</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_01/11/2018-12:40:42</t>
+    <t>TaskName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,22 +393,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1424184-5EE2-4BB2-B5FB-6C33B2F49EA9}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assign Task Test Case
</commit_message>
<xml_diff>
--- a/SCTestData/data.xlsx
+++ b/SCTestData/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FormName</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>AUTO_TOOL_KAT_TASK_01/11/2018-15:40:16</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-10:47:56</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-11:19:37</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-11:24:17</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-11:29:11</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-11:31:25</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_TASK_02/11/2018-11:37:10</t>
   </si>
 </sst>
 </file>
@@ -418,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 20 November
</commit_message>
<xml_diff>
--- a/SCTestData/data.xlsx
+++ b/SCTestData/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Data\SafetyChain-Test-Automation-Katalon\SCTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD340B-314C-4505-B23B-944CA6BB4078}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98718DFC-728D-4C69-B61B-657E3DBA93AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{46E2E1DA-1FC9-488C-935C-41E78C701628}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>FormName</t>
   </si>
@@ -41,61 +41,349 @@
     <t>AUTO_TOOL_KAT_TASK_13/11/2018-10:31:01</t>
   </si>
   <si>
-    <t>AUTO_TOOL_KAT_FORM_14/11/2018-13:07:31</t>
-  </si>
-  <si>
     <t>DocumentName1</t>
   </si>
   <si>
     <t>DocumentName2</t>
   </si>
   <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-12:25:36</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-12:25:36</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-12:32:43</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-12:32:43</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-12:41:41</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-12:41:41</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-13:54:53</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-13:54:53</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-14:06:42</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-14:06:42</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-14:39:05</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-14:39:05</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-14:47:45</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-14:47:45</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-14:54:59</t>
-  </si>
-  <si>
-    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-14:54:59</t>
+    <t>AUTO_TOOL_KAT_DOCUMENT_15/11/2018-15:49:06</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_15/11/2018-15:49:06</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_15/11/2018-17:20:55</t>
+  </si>
+  <si>
+    <t>TaskNameDMS</t>
+  </si>
+  <si>
+    <t>DocumentName3</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-10:57:07</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-10:57:07</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-10:57:07</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-10:58:15</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-10:58:15</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-10:58:15</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:02:01</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:02:01</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:02:01</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:08:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:08:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:08:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:26:53</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:26:53</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:26:53</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:44:39</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:44:39</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENTTASK16/11/2018-11:44:39</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:44:39</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:46:20</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:46:20</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENTTASK16/11/2018-11:46:20</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:46:20</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:50:19</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:50:19</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENTTASK16/11/2018-11:50:19</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:50:19</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-11:53:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT1_16/11/2018-11:53:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENTTASK16/11/2018-11:53:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-11:53:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_16/11/2018-12:21:52</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_16/11/2018-14:34:41</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_RESTORE_DOCUMENT16/11/2018-14:34:41</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENTTASK16/11/2018-14:34:41</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_16/11/2018-14:34:41</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-14:51:48</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-14:56:49</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-14:58:09</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-15:09:07</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-15:12:14</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-15:18:15</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-15:20:14</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-15:24:56</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-16:06:21</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:01:16</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:03:37</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:04:58</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:07:28</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:09:38</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:11:27</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:14:47</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:18:10</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:22:13</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-17:58:46</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-18:02:02</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-18:02:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-18:06:36</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_16/11/2018-18:14:03</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:23:01</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:24:50</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:28:14</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:29:49</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:35:16</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:37:39</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:49:08</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:53:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:55:18</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-10:58:28</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:01:46</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:05:55</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:13:14</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:16:15</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:22:04</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:34:51</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:36:30</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:38:20</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:40:42</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:42:13</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:45:36</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:47:06</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-11:52:19</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:02:40</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:05:29</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:07:26</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:17:57</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:19:02</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:20:29</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:28:02</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:36:01</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:39:42</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-12:42:43</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-13:24:31</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-13:26:04</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-13:30:46</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:26:49</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:29:14</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:42:41</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:45:48</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:47:08</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:49:06</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-14:50:57</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-15:00:27</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_FORM_ON_19/11/2018-15:02:32</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DOCUMENT_ON_19/11/2018-16:47:09</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_RESTORE_DOCUMENT_ON_19/11/2018-16:47:09</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_ASSIGN_TASK_DOCUMENT_ON_19/11/2018-16:47:09</t>
+  </si>
+  <si>
+    <t>AUTO_TOOL_KAT_DMS_TASK_ON_19/11/2018-16:47:09</t>
   </si>
 </sst>
 </file>
@@ -448,15 +736,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1424184-5EE2-4BB2-B5FB-6C33B2F49EA9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,24 +752,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>